<commit_message>
modifiche file train.py, files di utils e aggiunta note encoding.asp
</commit_message>
<xml_diff>
--- a/utils/registro_componenti.xlsx
+++ b/utils/registro_componenti.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95E9279-DD9C-4804-920B-62833265A8F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29553C22-996F-4623-827D-1A47705F75FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="ECB_Distinta SEF Articoli " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ECB_Distinta SEF Articoli '!$A$1:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ECB_Distinta SEF Articoli '!$A$1:$I$105</definedName>
     <definedName name="Filter_Databese" localSheetId="0" hidden="1">'ECB_Distinta SEF Articoli '!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1303,10 +1303,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3837,14 +3837,30 @@
     </row>
     <row r="94" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="15"/>
-      <c r="H94" s="16"/>
-      <c r="I94" s="17"/>
+      <c r="B94" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G94" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I94" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
@@ -3855,16 +3871,16 @@
         <v>29</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="G95" s="15" t="s">
-        <v>203</v>
+        <v>19</v>
       </c>
       <c r="H95" s="16" t="s">
         <v>20</v>
@@ -3882,13 +3898,13 @@
         <v>29</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>204</v>
+        <v>33</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>205</v>
+        <v>34</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>206</v>
+        <v>35</v>
       </c>
       <c r="G96" s="15" t="s">
         <v>19</v>
@@ -3906,16 +3922,16 @@
         <v>199</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="G97" s="15" t="s">
         <v>19</v>
@@ -3933,19 +3949,19 @@
         <v>199</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>207</v>
+        <v>102</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="H98" s="16" t="s">
         <v>20</v>
@@ -3960,19 +3976,19 @@
         <v>199</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>102</v>
+        <v>208</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>105</v>
+        <v>211</v>
       </c>
       <c r="G99" s="15" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="H99" s="16" t="s">
         <v>20</v>
@@ -3990,13 +4006,13 @@
         <v>208</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="G100" s="15" t="s">
         <v>19</v>
@@ -4014,22 +4030,22 @@
         <v>199</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>213</v>
+        <v>134</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="H101" s="16" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="I101" s="17">
         <v>1</v>
@@ -4041,25 +4057,25 @@
         <v>199</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="I102" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -4071,22 +4087,22 @@
         <v>152</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>138</v>
+        <v>215</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>141</v>
+        <v>218</v>
       </c>
       <c r="H103" s="16" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="I103" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -4098,16 +4114,16 @@
         <v>152</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>216</v>
+        <v>144</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>217</v>
+        <v>145</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="H104" s="16" t="s">
         <v>20</v>
@@ -4125,53 +4141,26 @@
         <v>152</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G105" s="15" t="s">
         <v>141</v>
       </c>
       <c r="H105" s="16" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="I105" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="9"/>
-      <c r="B106" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D106" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E106" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G106" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="H106" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="I106" s="17">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I5" xr:uid="{0460231C-5DD9-40C4-9927-92B4E3DBEF94}">
+  <autoFilter ref="A1:I105" xr:uid="{0460231C-5DD9-40C4-9927-92B4E3DBEF94}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I96">
       <sortCondition ref="C1:C5"/>
     </sortState>

</xml_diff>